<commit_message>
refactor: update detective texts and improve descriptions in main_obras.csv
</commit_message>
<xml_diff>
--- a/src/data/Datos Banksy (1).xlsx
+++ b/src/data/Datos Banksy (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dafyd\Documents\Escuela\2024\semestre 2\visualizacion\VD - Final (Banksy)\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91785B68-F384-4851-B453-3F750F2D8C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1793B5FD-8926-4E1A-9E46-95E9AAA79873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -895,37 +895,9 @@
     <t xml:space="preserve">Texto </t>
   </si>
   <si>
-    <t>Ubicada en Jerusalén, esta obra de Banksy representa la esperanza en un entorno marcado por el conflicto. Muestra a un manifestante, en posición de arrojar un cóctel molotov, pero que en su lugar sostiene un ramo de flores. El contraste simboliza el anhelo de cambio pacífico en una región plagada de violencia. En el contexto de Israel y Palestina, Banksy destaca cómo la lucha puede trascender la violencia y centrarse en mensajes de paz.</t>
-  </si>
-  <si>
-    <t>Instalada en Disneyland en 2006, esta obra crítica muestra una figura inflable vestida como un prisionero de Guantánamo. Creada en el contexto de denuncias sobre torturas y abusos en esta prisión estadounidense, la obra denuncia la hipocresía de los derechos humanos en un país que proyecta una imagen de libertad y democracia. Colocar esta obra en un parque de atracciones resalta el contraste entre la diversión y la dura realidad de los prisioneros.</t>
-  </si>
-  <si>
-    <t>Pintada en el muro de Cisjordania, esta obra representa la esperanza infantil en medio de un entorno hostil. Una niña es elevada por globos, como símbolo de escape y libertad. En el contexto de la ocupación israelí y las restricciones a los palestinos, la obra sugiere el deseo de superar las barreras físicas y emocionales. Es una metáfora visual del sueño de una infancia sin muros.</t>
-  </si>
-  <si>
-    <t>Creada en Toronto, esta obra critica la alienación moderna en un mundo hiperdigitalizado. A pesar de la hiperconexión en redes sociales, la obra refleja el desinterés genuino por las personas reales. En un momento donde la tecnología dominaba la interacción humana, Banksy usa esta pieza para señalar cómo las conexiones humanas se han reducido a transacciones superficiales.</t>
-  </si>
-  <si>
-    <t>Una reinterpretación de la obra de Monet que incorpora carros de supermercado y conos de tráfico flotando en un estanque. Esta pintura al óleo critica el impacto del consumismo en la naturaleza. En la Inglaterra de 2005, con una creciente preocupación por el cambio climático y la basura, Banksy transforma un paisaje idílico en una alegoría del descuido humano hacia el medio ambiente.</t>
-  </si>
-  <si>
-    <t>Esta obra, ubicada en Calais, Francia, muestra al hijo de un migrante como un símbolo de esperanza y humanidad. Realizada durante la crisis migratoria europea de 2015, Banksy visibiliza la lucha de los refugiados sirios por encontrar un hogar seguro. Con un chaleco salvavidas y una bengala, la obra destaca la valentía y desesperación de aquellos que arriesgan todo por sobrevivir.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pintada directamente sobre el muro de Cisjordania, esta obra muestra ventanas hacia paisajes paradisíacos. En el contexto de la ocupación israelí, el muro representa la división y la opresión. Banksy transforma este símbolo de separación en un acto de resistencia visual, sugiriendo un mundo donde las barreras físicas y sociales pueden ser superadas.
-Pintada directamente sobre el muro de Cisjordania, esta obra muestra ventanas hacia paisajes paradisíacos. En el contexto de la ocupación israelí, el muro representa la división y la opresión. Banksy transforma este símbolo de separación en un acto de resistencia visual, sugiriendo un mundo donde las barreras físicas y sociales pueden ser superadas.
-Pintada directamente sobre el muro de Cisjordania, esta obra muestra ventanas hacia paisajes paradisíacos. En el contexto de la ocupación israelí, el muro representa la división y la opresión. Banksy transforma este símbolo de separación en un acto de resistencia visual, sugiriendo un mundo donde las barreras físicas y sociales pueden ser superadas.
-Pintada directamente sobre el muro de Cisjordania, esta obra muestra ventanas hacia paisajes paradisíacos. En el contexto de la ocupación israelí, el muro representa la división y la opresión. Banksy transforma este símbolo de separación en un acto de resistencia visual, sugiriendo un mundo donde las barreras físicas y sociales pueden ser superadas.
-</t>
-  </si>
-  <si>
     <t>Ubicada en Nueva York, esta obra es una sátira sobre el consumismo. En un contexto donde el capitalismo prometía felicidad a través de bienes materiales, Banksy muestra cómo el sistema no puede cumplir con esas expectativas. Es un recordatorio de que la búsqueda constante de un "estilo de vida ideal" es insostenible y alienante.</t>
   </si>
   <si>
-    <t>Esta obra muestra a personas arrodilladas como si rezaran ante un cartel de "Sale Ends Today". Realizada en una época de obsesión con el consumismo, refleja cómo las ofertas y rebajas se han convertido en una suerte de religión moderna. En un mundo donde la identidad a menudo está definida por lo que compramos, Banksy critica la devoción desmedida por lo material.</t>
-  </si>
-  <si>
     <t>Titulo</t>
   </si>
   <si>
@@ -944,10 +916,34 @@
     <t>Longitud</t>
   </si>
   <si>
-    <t>Esta obra ironiza sobre la percepción del graffiti como una amenaza al sistema y resalta cómo el arte callejero es reprimido porque desafía la norma. En la Inglaterra de su tiempo, con leyes estrictas contra el vandalismo, Banksy señala que cualquier forma de cambio auténtico sería automáticamente criminalizada por el poder establecido.</t>
-  </si>
-  <si>
     <t>La obra es una crítica al poder y al control, con el mono como símbolo de los marginados y oprimidos. La frase sugiere que aquellos que actualmente no tienen poder algún día tomarán el control, invirtiendo el status quo.</t>
+  </si>
+  <si>
+    <t>Estamos en Jerusalén. Banksy aboga fuertemente por la paz y Medio Oriente es centro de muchas de sus obras que hacen alusión a esta causa. El contraste entre la pose violenta del manifestante, y el ramo de flores simboliza el anhelo de cambio pacífico en una región plagada de violencia.</t>
+  </si>
+  <si>
+    <t>Estamos en Disneyland, California. ¡Qué lugar para una obra de este estilo! Vaya que hace llegar su mensaje. Esta obra crítica muestra una figura inflable vestida como un prisionero de Guantánamo. Denuncia la hipocresía de los derechos humanos en un país que proyecta una imagen de libertad y democracia.</t>
+  </si>
+  <si>
+    <t>Ubicada en Londres, esta obra ironiza sobre la percepción del graffiti como una amenaza al sistema. Referencia a una cita de Emma Goldman y resalta cómo el arte callejero es reprimido porque desafía la norma.</t>
+  </si>
+  <si>
+    <t>Llegamos a Toronto. Esta obra critica la alienación moderna en un mundo hiperdigitalizado. A pesar de la hiperconexión en redes sociales, la obra refleja el desinterés genuino por las personas reales.</t>
+  </si>
+  <si>
+    <t>Pintada en el muro de Cisjordania, esta obra representa la esperanza infantil en medio de un entorno hostil. Una niña es elevada por globos, como símbolo de escape y libertad.</t>
+  </si>
+  <si>
+    <t>Localizada en Londres, esta reinterpretación de la obra de Monet critica el impacto del consumismo en la naturaleza. Banksy transforma un paisaje idílico en una alegoría del descuido humano hacia el medio ambiente.</t>
+  </si>
+  <si>
+    <t>¡Francia, oh là là! Ubicada en Calais, la obra muestra al hijo de un migrante como un símbolo de esperanza y humanidad. Con un chaleco salvavidas y una bengala, Banksy visibiliza la lucha de los refugiados sirios por encontrar un hogar seguro.</t>
+  </si>
+  <si>
+    <t>Pintada directamente sobre el muro de Cisjordania, esta obra muestra ventanas hacia paisajes paradisíacos. Banksy transforma este símbolo de separación en un acto de resistencia visual, sugiriendo un mundo donde las barreras físicas y sociales pueden ser superadas.</t>
+  </si>
+  <si>
+    <t>A nuestro artista misterioso le gusta Nueva York. Es la ciudad por excelencia para criticar al capitalismo salvaje. Esta obra muestra a personas arrodilladas como si rezaran ante un cartel de "Sale Ends Today". Banksy critica la devoción desmedida por lo material y refleja cómo las ofertas y rebajas se han convertido en una suerte de religión moderna.</t>
   </si>
 </sst>
 </file>
@@ -1388,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J69" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M74" sqref="M74:Z74"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="75" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M113" sqref="M113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,16 +1407,16 @@
   <sheetData>
     <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>61</v>
@@ -1432,13 +1428,13 @@
         <v>58</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
@@ -1754,7 +1750,7 @@
         <v>106</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -2035,7 +2031,7 @@
         <v>113</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
@@ -2469,7 +2465,7 @@
         <v>124</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
@@ -2523,7 +2519,7 @@
         <v>125</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
@@ -2577,7 +2573,7 @@
         <v>126</v>
       </c>
       <c r="M29" s="9" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
@@ -3505,7 +3501,7 @@
         <v>225</v>
       </c>
       <c r="M53" s="9" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
@@ -4129,7 +4125,7 @@
         <v>241</v>
       </c>
       <c r="M69" s="9" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="N69" s="9"/>
       <c r="O69" s="9"/>
@@ -4335,7 +4331,7 @@
         <v>246</v>
       </c>
       <c r="M74" s="9" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="N74" s="9"/>
       <c r="O74" s="9"/>
@@ -4883,7 +4879,7 @@
         <v>260</v>
       </c>
       <c r="M88" s="9" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="N88" s="9"/>
       <c r="O88" s="9"/>
@@ -5089,7 +5085,7 @@
         <v>265</v>
       </c>
       <c r="M93" s="9" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="N93" s="9"/>
       <c r="O93" s="9"/>
@@ -5827,7 +5823,7 @@
         <v>284</v>
       </c>
       <c r="M112" s="9" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="N112" s="9"/>
       <c r="O112" s="9"/>
@@ -5998,17 +5994,17 @@
   </sheetData>
   <autoFilter ref="I1:I116" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="11">
-    <mergeCell ref="M9:Y9"/>
-    <mergeCell ref="M16:Y16"/>
-    <mergeCell ref="M27:Z27"/>
-    <mergeCell ref="M28:Z28"/>
-    <mergeCell ref="M29:Z29"/>
     <mergeCell ref="M53:Z53"/>
     <mergeCell ref="M69:Z69"/>
     <mergeCell ref="M88:Z88"/>
     <mergeCell ref="M93:Z93"/>
     <mergeCell ref="M112:Z112"/>
     <mergeCell ref="M74:Z74"/>
+    <mergeCell ref="M9:Y9"/>
+    <mergeCell ref="M16:Y16"/>
+    <mergeCell ref="M27:Z27"/>
+    <mergeCell ref="M28:Z28"/>
+    <mergeCell ref="M29:Z29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L28" r:id="rId1" xr:uid="{F2CD6687-F296-4833-8C92-02DE1AE023E3}"/>

</xml_diff>